<commit_message>
Fixed web app UI
</commit_message>
<xml_diff>
--- a/ContactsWebApp/contacts_sample.xlsx
+++ b/ContactsWebApp/contacts_sample.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhavedula/Desktop/Glome/Contacts Web App/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhavedula/Desktop/Glome/ContactsWebApp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{966A351E-5284-334E-9B33-EE3C96E8299D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED3293FA-A0B7-9A44-B8A9-2E612B12C3CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{022DB5FF-A171-504C-85A2-F77172F047CA}"/>
   </bookViews>
@@ -42,16 +42,16 @@
     <t>Language</t>
   </si>
   <si>
-    <t>Abha Vedula</t>
-  </si>
-  <si>
-    <t>Sonali Dane</t>
-  </si>
-  <si>
     <t>French</t>
   </si>
   <si>
     <t>Arabic</t>
+  </si>
+  <si>
+    <t>Nikita Dane</t>
+  </si>
+  <si>
+    <t>Daphne Fong</t>
   </si>
 </sst>
 </file>
@@ -406,10 +406,13 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -424,24 +427,24 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>1111111111</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
-      </c>
-      <c r="B2">
-        <v>123456789</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>2222222222</v>
+      </c>
+      <c r="C3" t="s">
         <v>4</v>
-      </c>
-      <c r="B3">
-        <v>987654321</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>